<commit_message>
Added few more columns.
</commit_message>
<xml_diff>
--- a/ClientResearch/Shortlisting Potential Asian Clients.xlsx
+++ b/ClientResearch/Shortlisting Potential Asian Clients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cubes\OneDrive\CubeStatistica\Business-Development\ClientResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AF112E-32CD-4D7C-9AA7-3AF9C1E04D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E350390B-C39D-4D43-A1FA-1FEEE556A0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9A972389-D95F-EB41-AA28-F2A53DE7B95C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>international companies w/ local branches</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>Short_Listed</t>
+  </si>
+  <si>
+    <t>International_Company</t>
+  </si>
+  <si>
+    <t>Strictly_Local_Company</t>
+  </si>
+  <si>
+    <t>Country_Of_Origin????</t>
   </si>
 </sst>
 </file>
@@ -514,21 +523,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9992C808-5773-D54B-B480-464DC3743478}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.69921875" customWidth="1"/>
     <col min="2" max="2" width="34.296875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="21.19921875" customWidth="1"/>
-    <col min="5" max="5" width="15.59765625" customWidth="1"/>
+    <col min="3" max="7" width="21.19921875" customWidth="1"/>
+    <col min="8" max="8" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -539,19 +548,28 @@
         <v>26</v>
       </c>
       <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -561,11 +579,16 @@
       <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="b">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -575,11 +598,14 @@
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="b">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -590,8 +616,11 @@
         <v>16</v>
       </c>
       <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -602,8 +631,11 @@
         <v>16</v>
       </c>
       <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -614,8 +646,11 @@
         <v>16</v>
       </c>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -626,8 +661,11 @@
         <v>16</v>
       </c>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -638,8 +676,11 @@
         <v>16</v>
       </c>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -650,8 +691,11 @@
         <v>17</v>
       </c>
       <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -662,8 +706,11 @@
         <v>17</v>
       </c>
       <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -674,8 +721,11 @@
         <v>17</v>
       </c>
       <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -686,8 +736,11 @@
         <v>17</v>
       </c>
       <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -698,8 +751,11 @@
         <v>17</v>
       </c>
       <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
@@ -710,8 +766,11 @@
         <v>18</v>
       </c>
       <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>22</v>
       </c>
@@ -722,6 +781,9 @@
         <v>21</v>
       </c>
       <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B9 A5:A12">

</xml_diff>